<commit_message>
update RMD and basics and phasing switch
Phasing now TRUE/FALSE
updated vignette for basics
</commit_message>
<xml_diff>
--- a/vignettes/BS2017SS.xlsx
+++ b/vignettes/BS2017SS.xlsx
@@ -10,8 +10,8 @@
     <sheet name="meta_data" sheetId="1" r:id="rId1"/>
     <sheet name="control" sheetId="2" r:id="rId2"/>
     <sheet name="fleet_control" sheetId="3" r:id="rId3"/>
-    <sheet name="srv_biom" sheetId="4" r:id="rId4"/>
-    <sheet name="fsh_biom" sheetId="5" r:id="rId5"/>
+    <sheet name="index_data" sheetId="4" r:id="rId4"/>
+    <sheet name="catch_data" sheetId="5" r:id="rId5"/>
     <sheet name="comp_data" sheetId="6" r:id="rId6"/>
     <sheet name="emp_sel" sheetId="7" r:id="rId7"/>
     <sheet name="NByageFixed" sheetId="8" r:id="rId8"/>
@@ -25,7 +25,7 @@
     <sheet name="bioenergetics_control" sheetId="16" r:id="rId16"/>
     <sheet name="env_data" sheetId="17" r:id="rId17"/>
     <sheet name="Pyrs" sheetId="18" r:id="rId18"/>
-    <sheet name="UobsWtAge" sheetId="19" r:id="rId19"/>
+    <sheet name="stom_prop_data" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -788,12 +788,12 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Acuumulation_age_lower</t>
+          <t>Comp_loglike</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Ages below this will be grouped to this age for composition data. For example, if set to 2, comp data for age 2 will include 1 and 2 year olds.</t>
+          <t>Composition data distribution (0 = multinomial; 1 = dirichlet-multinomial)</t>
         </is>
       </c>
     </row>
@@ -823,12 +823,12 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Acuumulation_age_upper</t>
+          <t>weight1_Numbers2</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Ages above this will be grouped to this age for composition data. For example, if set to 9 for a species with 10 ages, comp data for age 9 will include 9 and 10 year olds.</t>
+          <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
         </is>
       </c>
     </row>
@@ -858,12 +858,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>weight1_Numbers2</t>
+          <t>Weight_index</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Is the observation in weight (kg) set as 1, if the observation is in numbers caught, set as 2</t>
+          <t>Weight-at-age (wt) index to use for calculation of derived quantities</t>
         </is>
       </c>
     </row>
@@ -893,12 +893,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Weight_index</t>
+          <t>Age_transition_index</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Weight-at-age (wt) index to use for calculation of derived quantities</t>
+          <t>Age transition matrix (e.g. growth trajectory) index to use for derived quantities to convert age to length</t>
         </is>
       </c>
     </row>
@@ -928,12 +928,12 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Age_transition_index</t>
+          <t>Q_index</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Age transition matrix (e.g. growth trajectory) index to use for derived quantities to convert age to length</t>
+          <t>index to use if catchability coefficients are to be set the same</t>
         </is>
       </c>
     </row>
@@ -963,12 +963,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Q_index</t>
+          <t>Estimate_q</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>index to use if catchability coefficients are to be set the same</t>
+          <t>Estimate catchability? (0 = fixed at prior; - 1 = Estimate single parameter; - 2 = Estimate single parameter with prior; - 3 = Estimate analytical q  from Ludwig and Walters 1994;  - 4 = Estimate power equation; - 5 - Linear equation log(q_y) = q_mu + beta * index_y)</t>
         </is>
       </c>
     </row>
@@ -998,12 +998,12 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Estimate_q</t>
+          <t>Q_prior</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Estimate catchability? (0 = fixed at prior; - 1 = Estimate single parameter; - 2 = Estimate single parameter with prior; - 3 = Estimate analytical q  from Ludwig and Walters 1994;  - 4 = Estimate power equation; - 5 - Linear equation log(q_y) = q_mu + beta * index_y)</t>
+          <t>Starting value or fixed value for catchability</t>
         </is>
       </c>
     </row>
@@ -1033,12 +1033,12 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Q_prior</t>
+          <t>Q_sd_prior</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Starting value or fixed value for catchability</t>
+          <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
         </is>
       </c>
     </row>
@@ -1068,12 +1068,12 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Q_sd_prior</t>
+          <t>Time_varying_q</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Variance of q prior: dnorm (log_q, log_q_prior, q_sd_prior)</t>
+          <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y. If "random_q" is selected in fit_mod, penalized deviates (1) and random walk parameters (4) will be treated as random effects.</t>
         </is>
       </c>
     </row>
@@ -1098,12 +1098,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Time_varying_q</t>
+          <t>Time_varying_q_sd_prior</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Wether a time-varying q should be estimated. 0 = no, 1 = penalized deviate, 3 = time blocks with no penalty; 4 = random walk from mean following Dorn 2018 (dnorm(q_y - q_y-1, 0, sigma). If Estimate_q = 5, this determines the environmental index to be used in the equation log(q_y) = q_mu + beta * index_y. If "random_q" is selected in fit_mod, penalized deviates (1) and random walk parameters (4) will be treated as random effects.</t>
+          <t>The sd to use for the random walk of time varying q if set to 1</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>srv_biom</t>
+          <t>index_data</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1128,12 +1128,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Time_varying_q_sd_prior</t>
+          <t>Estimate_survey_sd</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>The sd to use for the random walk of time varying q if set to 1</t>
+          <t>Estimate survey variance (0 = use CV from index_data, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>fsh_biom</t>
+          <t>catch_data</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1158,12 +1158,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Estimate_survey_sd</t>
+          <t>Survey_sd_prior</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Estimate survey variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
+          <t>Starting value to be used if Estimate_sigma_index = 1</t>
         </is>
       </c>
     </row>
@@ -1188,12 +1188,12 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Survey_sd_prior</t>
+          <t>Estimate_catch_sd</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Starting value to be used if Estimate_sigma_index = 1</t>
+          <t>Estimate fishery variance (0 = use CV from index_data, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
         </is>
       </c>
     </row>
@@ -1218,12 +1218,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Estimate_catch_sd</t>
+          <t>Catch_sd_prior</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Estimate fishery variance (0 = use CV from srv_biom, 1 = yes, 2 = analytically estimate following (Ludwig and Walters 1994)</t>
+          <t>Starting value to be used if Estimate_sigma_catch = 1</t>
         </is>
       </c>
     </row>
@@ -1248,12 +1248,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Catch_sd_prior</t>
+          <t>Comp_weights</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Starting value to be used if Estimate_sigma_catch = 1</t>
+          <t>Composition weights to be used for multinomial likelihood. These are multiplied. After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
         </is>
       </c>
     </row>
@@ -1278,12 +1278,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Comp_weights</t>
+          <t>Catch_units</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Composition weights to be used for multinomial likelihood. These are multiplied. After running model, these will update to McAllister &amp; Ianelli 1997 weights using the harmonic mean.</t>
+          <t>Units used for survey: 1 = kg; 2 = numbers</t>
         </is>
       </c>
     </row>
@@ -1308,12 +1308,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Catch_units</t>
+          <t>proj_F_prop</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Units used for survey: 1 = kg; 2 = numbers</t>
+          <t>The proportion of future fishing mortality assigned to this fleet</t>
         </is>
       </c>
     </row>
@@ -1334,16 +1334,6 @@
       <c r="E29" t="inlineStr">
         <is>
           <t>fleet_control</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>proj_F_prop</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>The proportion of future fishing mortality assigned to this fleet</t>
         </is>
       </c>
     </row>
@@ -12858,62 +12848,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>b</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0.005531354</v>
-      </c>
-      <c r="C2">
-        <v>3.04598</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0.003938607</v>
-      </c>
-      <c r="C3">
-        <v>3.256385</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>0.003638059</v>
-      </c>
-      <c r="C4">
-        <v>3.244794</v>
-      </c>
-    </row>
+    <row r="1" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -79229,7 +79170,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -79243,915 +79184,586 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pollock</t>
+          <t>Fleet_code</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cod</t>
+          <t>Fleet_type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>ATF</t>
+          <t>Species</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>BT_Pollock</t>
+          <t>Selectivity_index</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>BT_Cod</t>
+          <t>Selectivity</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>BT_ATF</t>
+          <t>Nselages</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>EIT_Pollock</t>
+          <t>Time_varying_sel</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Sel_sd_prior</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Age_first_selected</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Age_max_selected</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Comp_loglike</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Weight1_Numbers2</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Weight_index</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Age_transition_index</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Q_index</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Estimate_q</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Q_prior</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Q_sd_prior</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Time_varying_q</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Time_varying_q_sd_prior</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Estimate_index_sd</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Index_sd_prior</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Estimate_catch_sd</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Catch_sd_prior</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>Comp_weights</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>proj_F_prop</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fleet_code</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+          <t>Pollock</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>12.5</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>1</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Fleet_type</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+          <t>Cod</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3">
+        <v>12.5</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Species</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+          <t>ATF</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
+      <c r="I4">
+        <v>12.5</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Selectivity_index</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+          <t>BT_Pollock</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Selectivity</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+          <t>BT_Cod</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Nselages</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 8</t>
-        </is>
+          <t>BT_ATF</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 0</t>
+        </is>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Time_varying_sel</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
+          <t>EIT_Pollock</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+      <c r="P8">
+        <v>4</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0.001227838</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8" t="inlineStr">
         <is>
           <t xml:space="preserve"> 0</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Sel_sd_prior</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12.5</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.0</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.0</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.0</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Age_first_selected</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Accumatation_age_lower</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Accumatation_age_upper</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Weight1_Numbers2</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Weight_index</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Age_transition_index</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Q_index</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 2</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 3</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 4</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Estimate_q</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Q_prior</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>1.000000000</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>1.000000000</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>1.000000000</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>0.001227838</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Q_sd_prior</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Time_varying_q</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Time_varying_q_sd_prior</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Estimate_survey_sd</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Survey_sd_prior</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Estimate_catch_sd</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 0</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Catch_sd_prior</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Comp_weights</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>proj_F_prop</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>